<commit_message>
Upadte the create task page
</commit_message>
<xml_diff>
--- a/Client/bulkuploadtemplate.xlsx
+++ b/Client/bulkuploadtemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internal Project\TaggingTool\tagging-accelerator-v2\Client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9434A1-7180-4E7A-BE77-85B05FD17260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB96CF5B-8B98-45CA-B67B-7E217A9661B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{805BBC22-7CA0-42DA-BA74-FBC9517B3292}"/>
+    <workbookView xWindow="2460" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{805BBC22-7CA0-42DA-BA74-FBC9517B3292}"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk Upload" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Task_role</t>
   </si>
@@ -50,10 +50,19 @@
     <t>task_mediatype</t>
   </si>
   <si>
-    <t>task_filedata</t>
-  </si>
-  <si>
     <t>projectid</t>
+  </si>
+  <si>
+    <t>task_filename</t>
+  </si>
+  <si>
+    <t>task_filepath</t>
+  </si>
+  <si>
+    <t>task_title</t>
+  </si>
+  <si>
+    <t>profile_id</t>
   </si>
 </sst>
 </file>
@@ -405,39 +414,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98BCF83D-46A1-4121-9F9C-79373537CD6D}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>